<commit_message>
final push correction to q6
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjami\Documents\DA8\Projects\budget_lookups-cjpentecost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008CDBF0-63B7-4C43-BD0E-95306BCD1892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8C5BE8-50AE-4AE2-83A3-3684983ACAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -1029,10 +1029,10 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8837300</c:v>
+                  <c:v>3329000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8460963.1999999899</c:v>
+                  <c:v>2946071.21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1141,10 +1141,10 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9713300</c:v>
+                  <c:v>3390900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8991707.2399999909</c:v>
+                  <c:v>3051483.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1253,10 +1253,10 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9343000</c:v>
+                  <c:v>3345200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8766655.9100000001</c:v>
+                  <c:v>2946440.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2150,16 +2150,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1EB7F99E-A31D-4C13-982B-84C6998556D6}" name="Table2" displayName="Table2" ref="B87:B88" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="B87:B88" xr:uid="{1EB7F99E-A31D-4C13-982B-84C6998556D6}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0938D8D5-968C-4877-9F44-E6206DBDBED6}" name="Finance"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2459,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89:H90"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2538,11 +2528,11 @@
         <v>341243679.13</v>
       </c>
       <c r="D2">
-        <f>C2-B2</f>
+        <f t="shared" ref="D2:D33" si="0">C2-B2</f>
         <v>-15396420.870000005</v>
       </c>
       <c r="E2" s="5">
-        <f>IFERROR(D2/B2, 0)</f>
+        <f t="shared" ref="E2:E33" si="1">IFERROR(D2/B2, 0)</f>
         <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2">
@@ -2556,15 +2546,15 @@
         <v>346340810.81999999</v>
       </c>
       <c r="I2">
-        <f>H2-G2</f>
+        <f t="shared" ref="I2:I33" si="2">H2-G2</f>
         <v>-36344389.180000007</v>
       </c>
       <c r="J2" s="5">
-        <f>IFERROR(I2/G2, 0)</f>
+        <f t="shared" ref="J2:J33" si="3">IFERROR(I2/G2, 0)</f>
         <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
-        <f>RANK(J2,J:J,1)</f>
+        <f t="shared" ref="K2:K33" si="4">RANK(J2,J:J,1)</f>
         <v>10</v>
       </c>
       <c r="L2">
@@ -2574,15 +2564,15 @@
         <v>355279492.22999901</v>
       </c>
       <c r="N2">
-        <f>M2-L2</f>
+        <f t="shared" ref="N2:N33" si="5">M2-L2</f>
         <v>-21269107.770000994</v>
       </c>
       <c r="O2" s="5">
-        <f>IFERROR(N2/L2, 0)</f>
+        <f t="shared" ref="O2:O33" si="6">IFERROR(N2/L2, 0)</f>
         <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>RANK(O2,O:O,1)</f>
+        <f t="shared" ref="P2:P33" si="7">RANK(O2,O:O,1)</f>
         <v>14</v>
       </c>
     </row>
@@ -2597,15 +2587,15 @@
         <v>321214.59000000003</v>
       </c>
       <c r="D3">
-        <f>C3-B3</f>
+        <f t="shared" si="0"/>
         <v>-7585.4099999999744</v>
       </c>
       <c r="E3" s="5">
-        <f>IFERROR(D3/B3, 0)</f>
+        <f t="shared" si="1"/>
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f>RANK(E3,E:E,1)</f>
+        <f t="shared" ref="F3:F34" si="8">RANK(E3,E:E,1)</f>
         <v>22</v>
       </c>
       <c r="G3">
@@ -2615,15 +2605,15 @@
         <v>312433.70999999897</v>
       </c>
       <c r="I3">
-        <f>H3-G3</f>
+        <f t="shared" si="2"/>
         <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f>IFERROR(I3/G3, 0)</f>
+        <f t="shared" si="3"/>
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f>RANK(J3,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="L3">
@@ -2633,15 +2623,15 @@
         <v>322263.03999999998</v>
       </c>
       <c r="N3">
-        <f>M3-L3</f>
+        <f t="shared" si="5"/>
         <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f>IFERROR(N3/L3, 0)</f>
+        <f t="shared" si="6"/>
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f>RANK(O3,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
     </row>
@@ -2656,15 +2646,15 @@
         <v>3115157.5599999898</v>
       </c>
       <c r="D4">
-        <f>C4-B4</f>
+        <f t="shared" si="0"/>
         <v>-15442.440000010189</v>
       </c>
       <c r="E4" s="5">
-        <f>IFERROR(D4/B4, 0)</f>
+        <f t="shared" si="1"/>
         <v>-4.9327413275443007E-3</v>
       </c>
       <c r="F4">
-        <f>RANK(E4,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>42</v>
       </c>
       <c r="G4">
@@ -2674,15 +2664,15 @@
         <v>3589693.2099999902</v>
       </c>
       <c r="I4">
-        <f>H4-G4</f>
+        <f t="shared" si="2"/>
         <v>-62606.790000009816</v>
       </c>
       <c r="J4" s="5">
-        <f>IFERROR(I4/G4, 0)</f>
+        <f t="shared" si="3"/>
         <v>-1.7141743558856015E-2</v>
       </c>
       <c r="K4">
-        <f>RANK(J4,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="L4">
@@ -2692,15 +2682,15 @@
         <v>3564983.04999999</v>
       </c>
       <c r="N4">
-        <f>M4-L4</f>
+        <f t="shared" si="5"/>
         <v>-97416.950000009965</v>
       </c>
       <c r="O4" s="5">
-        <f>IFERROR(N4/L4, 0)</f>
+        <f t="shared" si="6"/>
         <v>-2.6599210899959033E-2</v>
       </c>
       <c r="P4">
-        <f>RANK(O4,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
     </row>
@@ -2715,15 +2705,15 @@
         <v>6947552.6699999999</v>
       </c>
       <c r="D5">
-        <f>C5-B5</f>
+        <f t="shared" si="0"/>
         <v>-723147.33000000007</v>
       </c>
       <c r="E5" s="5">
-        <f>IFERROR(D5/B5, 0)</f>
+        <f t="shared" si="1"/>
         <v>-9.4273968477453174E-2</v>
       </c>
       <c r="F5">
-        <f>RANK(E5,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="G5">
@@ -2733,15 +2723,15 @@
         <v>7020609.3200000003</v>
       </c>
       <c r="I5">
-        <f>H5-G5</f>
+        <f t="shared" si="2"/>
         <v>-947690.6799999997</v>
       </c>
       <c r="J5" s="5">
-        <f>IFERROR(I5/G5, 0)</f>
+        <f t="shared" si="3"/>
         <v>-0.118932605449092</v>
       </c>
       <c r="K5">
-        <f>RANK(J5,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="L5">
@@ -2751,15 +2741,15 @@
         <v>7497322.9100000001</v>
       </c>
       <c r="N5">
-        <f>M5-L5</f>
+        <f t="shared" si="5"/>
         <v>-262277.08999999985</v>
       </c>
       <c r="O5" s="5">
-        <f>IFERROR(N5/L5, 0)</f>
+        <f t="shared" si="6"/>
         <v>-3.3800336357544182E-2</v>
       </c>
       <c r="P5">
-        <f>RANK(O5,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
     </row>
@@ -2774,15 +2764,15 @@
         <v>385908.52</v>
       </c>
       <c r="D6">
-        <f>C6-B6</f>
+        <f t="shared" si="0"/>
         <v>-23391.479999999981</v>
       </c>
       <c r="E6" s="5">
-        <f>IFERROR(D6/B6, 0)</f>
+        <f t="shared" si="1"/>
         <v>-5.7149963352064452E-2</v>
       </c>
       <c r="F6">
-        <f>RANK(E6,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="G6">
@@ -2792,15 +2782,15 @@
         <v>427758.64</v>
       </c>
       <c r="I6">
-        <f>H6-G6</f>
+        <f t="shared" si="2"/>
         <v>-741.35999999998603</v>
       </c>
       <c r="J6" s="5">
-        <f>IFERROR(I6/G6, 0)</f>
+        <f t="shared" si="3"/>
         <v>-1.7301283547257551E-3</v>
       </c>
       <c r="K6">
-        <f>RANK(J6,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
       <c r="L6">
@@ -2810,15 +2800,15 @@
         <v>445114.28999999899</v>
       </c>
       <c r="N6">
-        <f>M6-L6</f>
+        <f t="shared" si="5"/>
         <v>-85.710000001010485</v>
       </c>
       <c r="O6" s="5">
-        <f>IFERROR(N6/L6, 0)</f>
+        <f t="shared" si="6"/>
         <v>-1.925202156356929E-4</v>
       </c>
       <c r="P6">
-        <f>RANK(O6,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>39</v>
       </c>
     </row>
@@ -2833,15 +2823,15 @@
         <v>2946071.21</v>
       </c>
       <c r="D7">
-        <f>C7-B7</f>
+        <f t="shared" si="0"/>
         <v>-382928.79000000004</v>
       </c>
       <c r="E7" s="5">
-        <f>IFERROR(D7/B7, 0)</f>
+        <f t="shared" si="1"/>
         <v>-0.11502817362571344</v>
       </c>
       <c r="F7">
-        <f>RANK(E7,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="G7">
@@ -2851,15 +2841,15 @@
         <v>3051483.41</v>
       </c>
       <c r="I7">
-        <f>H7-G7</f>
+        <f t="shared" si="2"/>
         <v>-339416.58999999985</v>
       </c>
       <c r="J7" s="5">
-        <f>IFERROR(I7/G7, 0)</f>
+        <f t="shared" si="3"/>
         <v>-0.10009631366303927</v>
       </c>
       <c r="K7">
-        <f>RANK(J7,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L7">
@@ -2869,15 +2859,15 @@
         <v>2946440.08</v>
       </c>
       <c r="N7">
-        <f>M7-L7</f>
+        <f t="shared" si="5"/>
         <v>-398759.91999999993</v>
       </c>
       <c r="O7" s="5">
-        <f>IFERROR(N7/L7, 0)</f>
+        <f t="shared" si="6"/>
         <v>-0.11920361114432618</v>
       </c>
       <c r="P7">
-        <f>RANK(O7,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
@@ -2892,15 +2882,15 @@
         <v>1315623.30999999</v>
       </c>
       <c r="D8">
-        <f>C8-B8</f>
+        <f t="shared" si="0"/>
         <v>-236476.69000000996</v>
       </c>
       <c r="E8" s="5">
-        <f>IFERROR(D8/B8, 0)</f>
+        <f t="shared" si="1"/>
         <v>-0.15235918433091292</v>
       </c>
       <c r="F8">
-        <f>RANK(E8,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G8">
@@ -2910,15 +2900,15 @@
         <v>1383905.98999999</v>
       </c>
       <c r="I8">
-        <f>H8-G8</f>
+        <f t="shared" si="2"/>
         <v>-206794.01000001002</v>
       </c>
       <c r="J8" s="5">
-        <f>IFERROR(I8/G8, 0)</f>
+        <f t="shared" si="3"/>
         <v>-0.13000189224870184</v>
       </c>
       <c r="K8">
-        <f>RANK(J8,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L8">
@@ -2928,15 +2918,15 @@
         <v>1337735.3199999901</v>
       </c>
       <c r="N8">
-        <f>M8-L8</f>
+        <f t="shared" si="5"/>
         <v>-241564.68000000995</v>
       </c>
       <c r="O8" s="5">
-        <f>IFERROR(N8/L8, 0)</f>
+        <f t="shared" si="6"/>
         <v>-0.15295680364719175</v>
       </c>
       <c r="P8">
-        <f>RANK(O8,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
@@ -2951,15 +2941,15 @@
         <v>8952825.2799999993</v>
       </c>
       <c r="D9">
-        <f>C9-B9</f>
+        <f t="shared" si="0"/>
         <v>-396574.72000000067</v>
       </c>
       <c r="E9" s="5">
-        <f>IFERROR(D9/B9, 0)</f>
+        <f t="shared" si="1"/>
         <v>-4.2417130511048909E-2</v>
       </c>
       <c r="F9">
-        <f>RANK(E9,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="G9">
@@ -2969,15 +2959,15 @@
         <v>9929059.5199999996</v>
       </c>
       <c r="I9">
-        <f>H9-G9</f>
+        <f t="shared" si="2"/>
         <v>-1144640.4800000004</v>
       </c>
       <c r="J9" s="5">
-        <f>IFERROR(I9/G9, 0)</f>
+        <f t="shared" si="3"/>
         <v>-0.10336567542917005</v>
       </c>
       <c r="K9">
-        <f>RANK(J9,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="L9">
@@ -2987,15 +2977,15 @@
         <v>9993599.52999999</v>
       </c>
       <c r="N9">
-        <f>M9-L9</f>
+        <f t="shared" si="5"/>
         <v>-796900.47000000998</v>
       </c>
       <c r="O9" s="5">
-        <f>IFERROR(N9/L9, 0)</f>
+        <f t="shared" si="6"/>
         <v>-7.3852043000788653E-2</v>
       </c>
       <c r="P9">
-        <f>RANK(O9,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
     </row>
@@ -3010,15 +3000,15 @@
         <v>407090.37</v>
       </c>
       <c r="D10">
-        <f>C10-B10</f>
+        <f t="shared" si="0"/>
         <v>-36209.630000000005</v>
       </c>
       <c r="E10" s="5">
-        <f>IFERROR(D10/B10, 0)</f>
+        <f t="shared" si="1"/>
         <v>-8.1681998646514792E-2</v>
       </c>
       <c r="F10">
-        <f>RANK(E10,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="G10">
@@ -3028,15 +3018,15 @@
         <v>467907.84000000003</v>
       </c>
       <c r="I10">
-        <f>H10-G10</f>
+        <f t="shared" si="2"/>
         <v>-27292.159999999974</v>
       </c>
       <c r="J10" s="5">
-        <f>IFERROR(I10/G10, 0)</f>
+        <f t="shared" si="3"/>
         <v>-5.5113408723747932E-2</v>
       </c>
       <c r="K10">
-        <f>RANK(J10,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="L10">
@@ -3046,15 +3036,15 @@
         <v>478318.92</v>
       </c>
       <c r="N10">
-        <f>M10-L10</f>
+        <f t="shared" si="5"/>
         <v>-9181.0800000000163</v>
       </c>
       <c r="O10" s="5">
-        <f>IFERROR(N10/L10, 0)</f>
+        <f t="shared" si="6"/>
         <v>-1.883298461538465E-2</v>
       </c>
       <c r="P10">
-        <f>RANK(O10,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
     </row>
@@ -3069,15 +3059,15 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>C11-B11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="5">
-        <f>IFERROR(D11/B11, 0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <f>RANK(E11,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>47</v>
       </c>
       <c r="G11">
@@ -3087,15 +3077,15 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <f>H11-G11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J11" s="5">
-        <f>IFERROR(I11/G11, 0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K11">
-        <f>RANK(J11,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="L11">
@@ -3105,15 +3095,15 @@
         <v>63771.91</v>
       </c>
       <c r="N11">
-        <f>M11-L11</f>
+        <f t="shared" si="5"/>
         <v>-311228.08999999997</v>
       </c>
       <c r="O11" s="5">
-        <f>IFERROR(N11/L11, 0)</f>
+        <f t="shared" si="6"/>
         <v>-0.82994157333333329</v>
       </c>
       <c r="P11">
-        <f>RANK(O11,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3128,15 +3118,15 @@
         <v>4066595.33</v>
       </c>
       <c r="D12">
-        <f>C12-B12</f>
+        <f t="shared" si="0"/>
         <v>-214304.66999999993</v>
       </c>
       <c r="E12" s="5">
-        <f>IFERROR(D12/B12, 0)</f>
+        <f t="shared" si="1"/>
         <v>-5.0060657805601608E-2</v>
       </c>
       <c r="F12">
-        <f>RANK(E12,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="G12">
@@ -3146,15 +3136,15 @@
         <v>4205555.5999999996</v>
       </c>
       <c r="I12">
-        <f>H12-G12</f>
+        <f t="shared" si="2"/>
         <v>-494844.40000000037</v>
       </c>
       <c r="J12" s="5">
-        <f>IFERROR(I12/G12, 0)</f>
+        <f t="shared" si="3"/>
         <v>-0.10527708280146378</v>
       </c>
       <c r="K12">
-        <f>RANK(J12,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="L12">
@@ -3164,15 +3154,15 @@
         <v>4371713.1399999997</v>
       </c>
       <c r="N12">
-        <f>M12-L12</f>
+        <f t="shared" si="5"/>
         <v>-306086.86000000034</v>
       </c>
       <c r="O12" s="5">
-        <f>IFERROR(N12/L12, 0)</f>
+        <f t="shared" si="6"/>
         <v>-6.5433934755654441E-2</v>
       </c>
       <c r="P12">
-        <f>RANK(O12,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -3187,15 +3177,15 @@
         <v>5772288.3300000001</v>
       </c>
       <c r="D13">
-        <f>C13-B13</f>
+        <f t="shared" si="0"/>
         <v>-75511.669999999925</v>
       </c>
       <c r="E13" s="5">
-        <f>IFERROR(D13/B13, 0)</f>
+        <f t="shared" si="1"/>
         <v>-1.2912833886247806E-2</v>
       </c>
       <c r="F13">
-        <f>RANK(E13,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>33</v>
       </c>
       <c r="G13">
@@ -3205,15 +3195,15 @@
         <v>5909077.9399999902</v>
       </c>
       <c r="I13">
-        <f>H13-G13</f>
+        <f t="shared" si="2"/>
         <v>-314622.06000000983</v>
       </c>
       <c r="J13" s="5">
-        <f>IFERROR(I13/G13, 0)</f>
+        <f t="shared" si="3"/>
         <v>-5.0552253482656594E-2</v>
       </c>
       <c r="K13">
-        <f>RANK(J13,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="L13">
@@ -3223,15 +3213,15 @@
         <v>6056976.6699999999</v>
       </c>
       <c r="N13">
-        <f>M13-L13</f>
+        <f t="shared" si="5"/>
         <v>-150323.33000000007</v>
       </c>
       <c r="O13" s="5">
-        <f>IFERROR(N13/L13, 0)</f>
+        <f t="shared" si="6"/>
         <v>-2.4217184605222895E-2</v>
       </c>
       <c r="P13">
-        <f>RANK(O13,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
     </row>
@@ -3246,15 +3236,15 @@
         <v>505017.37</v>
       </c>
       <c r="D14">
-        <f>C14-B14</f>
+        <f t="shared" si="0"/>
         <v>-6982.6300000000047</v>
       </c>
       <c r="E14" s="5">
-        <f>IFERROR(D14/B14, 0)</f>
+        <f t="shared" si="1"/>
         <v>-1.3637949218750009E-2</v>
       </c>
       <c r="F14">
-        <f>RANK(E14,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="G14">
@@ -3264,15 +3254,15 @@
         <v>524402.98</v>
       </c>
       <c r="I14">
-        <f>H14-G14</f>
+        <f t="shared" si="2"/>
         <v>-6097.0200000000186</v>
       </c>
       <c r="J14" s="5">
-        <f>IFERROR(I14/G14, 0)</f>
+        <f t="shared" si="3"/>
         <v>-1.1492968897266765E-2</v>
       </c>
       <c r="K14">
-        <f>RANK(J14,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="L14">
@@ -3282,15 +3272,15 @@
         <v>504989.88</v>
       </c>
       <c r="N14">
-        <f>M14-L14</f>
+        <f t="shared" si="5"/>
         <v>-21210.119999999995</v>
       </c>
       <c r="O14" s="5">
-        <f>IFERROR(N14/L14, 0)</f>
+        <f t="shared" si="6"/>
         <v>-4.0308095781071827E-2</v>
       </c>
       <c r="P14">
-        <f>RANK(O14,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
     </row>
@@ -3305,15 +3295,15 @@
         <v>156545919.90000001</v>
       </c>
       <c r="D15">
-        <f>C15-B15</f>
+        <f t="shared" si="0"/>
         <v>496819.90000000596</v>
       </c>
       <c r="E15" s="5">
-        <f>IFERROR(D15/B15, 0)</f>
+        <f t="shared" si="1"/>
         <v>3.1837408866824991E-3</v>
       </c>
       <c r="F15">
-        <f>RANK(E15,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>51</v>
       </c>
       <c r="G15">
@@ -3323,15 +3313,15 @@
         <v>175966389.24999899</v>
       </c>
       <c r="I15">
-        <f>H15-G15</f>
+        <f t="shared" si="2"/>
         <v>-8201410.7500010133</v>
       </c>
       <c r="J15" s="5">
-        <f>IFERROR(I15/G15, 0)</f>
+        <f t="shared" si="3"/>
         <v>-4.4532273014072019E-2</v>
       </c>
       <c r="K15">
-        <f>RANK(J15,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="L15">
@@ -3341,15 +3331,15 @@
         <v>184450910.84999901</v>
       </c>
       <c r="N15">
-        <f>M15-L15</f>
+        <f t="shared" si="5"/>
         <v>-4502589.1500009894</v>
       </c>
       <c r="O15" s="5">
-        <f>IFERROR(N15/L15, 0)</f>
+        <f t="shared" si="6"/>
         <v>-2.3829085727446114E-2</v>
       </c>
       <c r="P15">
-        <f>RANK(O15,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
     </row>
@@ -3364,15 +3354,15 @@
         <v>6522480.4599999897</v>
       </c>
       <c r="D16">
-        <f>C16-B16</f>
+        <f t="shared" si="0"/>
         <v>-78219.540000010282</v>
       </c>
       <c r="E16" s="5">
-        <f>IFERROR(D16/B16, 0)</f>
+        <f t="shared" si="1"/>
         <v>-1.1850188616360429E-2</v>
       </c>
       <c r="F16">
-        <f>RANK(E16,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
       <c r="G16">
@@ -3382,15 +3372,15 @@
         <v>7350464.0800000001</v>
       </c>
       <c r="I16">
-        <f>H16-G16</f>
+        <f t="shared" si="2"/>
         <v>-2035.9199999999255</v>
       </c>
       <c r="J16" s="5">
-        <f>IFERROR(I16/G16, 0)</f>
+        <f t="shared" si="3"/>
         <v>-2.769017341040361E-4</v>
       </c>
       <c r="K16">
-        <f>RANK(J16,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
       <c r="L16">
@@ -3400,15 +3390,15 @@
         <v>7397093</v>
       </c>
       <c r="N16">
-        <f>M16-L16</f>
+        <f t="shared" si="5"/>
         <v>-107</v>
       </c>
       <c r="O16" s="5">
-        <f>IFERROR(N16/L16, 0)</f>
+        <f t="shared" si="6"/>
         <v>-1.4464932677229222E-5</v>
       </c>
       <c r="P16">
-        <f>RANK(O16,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
     </row>
@@ -3423,15 +3413,15 @@
         <v>14439480.050000001</v>
       </c>
       <c r="D17">
-        <f>C17-B17</f>
+        <f t="shared" si="0"/>
         <v>-421319.94999999925</v>
       </c>
       <c r="E17" s="5">
-        <f>IFERROR(D17/B17, 0)</f>
+        <f t="shared" si="1"/>
         <v>-2.8351094826658003E-2</v>
       </c>
       <c r="F17">
-        <f>RANK(E17,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="G17">
@@ -3441,15 +3431,15 @@
         <v>14645233.51</v>
       </c>
       <c r="I17">
-        <f>H17-G17</f>
+        <f t="shared" si="2"/>
         <v>-664466.49000000022</v>
       </c>
       <c r="J17" s="5">
-        <f>IFERROR(I17/G17, 0)</f>
+        <f t="shared" si="3"/>
         <v>-4.3401666263871937E-2</v>
       </c>
       <c r="K17">
-        <f>RANK(J17,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="L17">
@@ -3459,15 +3449,15 @@
         <v>14346057.039999999</v>
       </c>
       <c r="N17">
-        <f>M17-L17</f>
+        <f t="shared" si="5"/>
         <v>-965742.96000000089</v>
       </c>
       <c r="O17" s="5">
-        <f>IFERROR(N17/L17, 0)</f>
+        <f t="shared" si="6"/>
         <v>-6.3071811282801551E-2</v>
       </c>
       <c r="P17">
-        <f>RANK(O17,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -3482,15 +3472,15 @@
         <v>2615303.8999999901</v>
       </c>
       <c r="D18">
-        <f>C18-B18</f>
+        <f t="shared" si="0"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="E18" s="5">
-        <f>IFERROR(D18/B18, 0)</f>
+        <f t="shared" si="1"/>
         <v>-5.4037002206391245E-2</v>
       </c>
       <c r="F18">
-        <f>RANK(E18,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="G18">
@@ -3500,15 +3490,15 @@
         <v>2671745.94</v>
       </c>
       <c r="I18">
-        <f>H18-G18</f>
+        <f t="shared" si="2"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="J18" s="5">
-        <f>IFERROR(I18/G18, 0)</f>
+        <f t="shared" si="3"/>
         <v>-6.6149619014330668E-2</v>
       </c>
       <c r="K18">
-        <f>RANK(J18,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="L18">
@@ -3518,15 +3508,15 @@
         <v>2535637.09</v>
       </c>
       <c r="N18">
-        <f>M18-L18</f>
+        <f t="shared" si="5"/>
         <v>-374962.91000000015</v>
       </c>
       <c r="O18" s="5">
-        <f>IFERROR(N18/L18, 0)</f>
+        <f t="shared" si="6"/>
         <v>-0.12882667147667154</v>
       </c>
       <c r="P18">
-        <f>RANK(O18,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
@@ -3541,15 +3531,15 @@
         <v>8460963.1999999899</v>
       </c>
       <c r="D19">
-        <f>C19-B19</f>
+        <f t="shared" si="0"/>
         <v>-376336.80000001006</v>
       </c>
       <c r="E19" s="5">
-        <f>IFERROR(D19/B19, 0)</f>
+        <f t="shared" si="1"/>
         <v>-4.258504294298146E-2</v>
       </c>
       <c r="F19">
-        <f>RANK(E19,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="G19">
@@ -3559,15 +3549,15 @@
         <v>8991707.2399999909</v>
       </c>
       <c r="I19">
-        <f>H19-G19</f>
+        <f t="shared" si="2"/>
         <v>-721592.76000000909</v>
       </c>
       <c r="J19" s="5">
-        <f>IFERROR(I19/G19, 0)</f>
+        <f t="shared" si="3"/>
         <v>-7.4289145810384635E-2</v>
       </c>
       <c r="K19">
-        <f>RANK(J19,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="L19">
@@ -3577,15 +3567,15 @@
         <v>8766655.9100000001</v>
       </c>
       <c r="N19">
-        <f>M19-L19</f>
+        <f t="shared" si="5"/>
         <v>-576344.08999999985</v>
       </c>
       <c r="O19" s="5">
-        <f>IFERROR(N19/L19, 0)</f>
+        <f t="shared" si="6"/>
         <v>-6.1687262121374278E-2</v>
       </c>
       <c r="P19">
-        <f>RANK(O19,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -3600,15 +3590,15 @@
         <v>124384360.159999</v>
       </c>
       <c r="D20">
-        <f>C20-B20</f>
+        <f t="shared" si="0"/>
         <v>-1539.8400010019541</v>
       </c>
       <c r="E20" s="5">
-        <f>IFERROR(D20/B20, 0)</f>
+        <f t="shared" si="1"/>
         <v>-1.2379538203300809E-5</v>
       </c>
       <c r="F20">
-        <f>RANK(E20,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>46</v>
       </c>
       <c r="G20">
@@ -3618,15 +3608,15 @@
         <v>131839624.37</v>
       </c>
       <c r="I20">
-        <f>H20-G20</f>
+        <f t="shared" si="2"/>
         <v>-9775.6299999952316</v>
       </c>
       <c r="J20" s="5">
-        <f>IFERROR(I20/G20, 0)</f>
+        <f t="shared" si="3"/>
         <v>-7.4142392760188761E-5</v>
       </c>
       <c r="K20">
-        <f>RANK(J20,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="L20">
@@ -3636,15 +3626,15 @@
         <v>130621283.53999899</v>
       </c>
       <c r="N20">
-        <f>M20-L20</f>
+        <f t="shared" si="5"/>
         <v>-116.46000100672245</v>
       </c>
       <c r="O20" s="5">
-        <f>IFERROR(N20/L20, 0)</f>
+        <f t="shared" si="6"/>
         <v>-8.9158438821450736E-7</v>
       </c>
       <c r="P20">
-        <f>RANK(O20,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>46</v>
       </c>
     </row>
@@ -3659,15 +3649,15 @@
         <v>22408587.5499999</v>
       </c>
       <c r="D21">
-        <f>C21-B21</f>
+        <f t="shared" si="0"/>
         <v>-1923512.4500000998</v>
       </c>
       <c r="E21" s="5">
-        <f>IFERROR(D21/B21, 0)</f>
+        <f t="shared" si="1"/>
         <v>-7.9052463618023094E-2</v>
       </c>
       <c r="F21">
-        <f>RANK(E21,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="G21">
@@ -3677,15 +3667,15 @@
         <v>22655993.629999999</v>
       </c>
       <c r="I21">
-        <f>H21-G21</f>
+        <f t="shared" si="2"/>
         <v>-1841406.370000001</v>
       </c>
       <c r="J21" s="5">
-        <f>IFERROR(I21/G21, 0)</f>
+        <f t="shared" si="3"/>
         <v>-7.5167420624229556E-2</v>
       </c>
       <c r="K21">
-        <f>RANK(J21,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="L21">
@@ -3695,15 +3685,15 @@
         <v>23434073.089999899</v>
       </c>
       <c r="N21">
-        <f>M21-L21</f>
+        <f t="shared" si="5"/>
         <v>-888926.91000010073</v>
       </c>
       <c r="O21" s="5">
-        <f>IFERROR(N21/L21, 0)</f>
+        <f t="shared" si="6"/>
         <v>-3.6546762734864152E-2</v>
       </c>
       <c r="P21">
-        <f>RANK(O21,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
     </row>
@@ -3718,15 +3708,15 @@
         <v>11412339.8799999</v>
       </c>
       <c r="D22">
-        <f>C22-B22</f>
+        <f t="shared" si="0"/>
         <v>-153660.12000009976</v>
       </c>
       <c r="E22" s="5">
-        <f>IFERROR(D22/B22, 0)</f>
+        <f t="shared" si="1"/>
         <v>-1.3285502334437123E-2</v>
       </c>
       <c r="F22">
-        <f>RANK(E22,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
       <c r="G22">
@@ -3736,15 +3726,15 @@
         <v>11791977.9699999</v>
       </c>
       <c r="I22">
-        <f>H22-G22</f>
+        <f t="shared" si="2"/>
         <v>-188722.03000009991</v>
       </c>
       <c r="J22" s="5">
-        <f>IFERROR(I22/G22, 0)</f>
+        <f t="shared" si="3"/>
         <v>-1.5752170574348738E-2</v>
       </c>
       <c r="K22">
-        <f>RANK(J22,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
       <c r="L22">
@@ -3754,15 +3744,15 @@
         <v>11934454.77</v>
       </c>
       <c r="N22">
-        <f>M22-L22</f>
+        <f t="shared" si="5"/>
         <v>-745.23000000044703</v>
       </c>
       <c r="O22" s="5">
-        <f>IFERROR(N22/L22, 0)</f>
+        <f t="shared" si="6"/>
         <v>-6.2439674240938325E-5</v>
       </c>
       <c r="P22">
-        <f>RANK(O22,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
     </row>
@@ -3777,15 +3767,15 @@
         <v>20036743.4099999</v>
       </c>
       <c r="D23">
-        <f>C23-B23</f>
+        <f t="shared" si="0"/>
         <v>-825956.59000010043</v>
       </c>
       <c r="E23" s="5">
-        <f>IFERROR(D23/B23, 0)</f>
+        <f t="shared" si="1"/>
         <v>-3.9590110100806722E-2</v>
       </c>
       <c r="F23">
-        <f>RANK(E23,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="G23">
@@ -3795,15 +3785,15 @@
         <v>21722126.219999898</v>
       </c>
       <c r="I23">
-        <f>H23-G23</f>
+        <f t="shared" si="2"/>
         <v>-961673.78000010177</v>
       </c>
       <c r="J23" s="5">
-        <f>IFERROR(I23/G23, 0)</f>
+        <f t="shared" si="3"/>
         <v>-4.2394738976719144E-2</v>
       </c>
       <c r="K23">
-        <f>RANK(J23,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="L23">
@@ -3813,15 +3803,15 @@
         <v>22619057.440000001</v>
       </c>
       <c r="N23">
-        <f>M23-L23</f>
+        <f t="shared" si="5"/>
         <v>-601242.55999999866</v>
       </c>
       <c r="O23" s="5">
-        <f>IFERROR(N23/L23, 0)</f>
+        <f t="shared" si="6"/>
         <v>-2.5892971236375011E-2</v>
       </c>
       <c r="P23">
-        <f>RANK(O23,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
     </row>
@@ -3836,15 +3826,15 @@
         <v>904969.19</v>
       </c>
       <c r="D24">
-        <f>C24-B24</f>
+        <f t="shared" si="0"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="E24" s="5">
-        <f>IFERROR(D24/B24, 0)</f>
+        <f t="shared" si="1"/>
         <v>-1.3334943305713101E-2</v>
       </c>
       <c r="F24">
-        <f>RANK(E24,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>31</v>
       </c>
       <c r="G24">
@@ -3854,15 +3844,15 @@
         <v>1067214.42</v>
       </c>
       <c r="I24">
-        <f>H24-G24</f>
+        <f t="shared" si="2"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="J24" s="5">
-        <f>IFERROR(I24/G24, 0)</f>
+        <f t="shared" si="3"/>
         <v>-4.087856565111897E-2</v>
       </c>
       <c r="K24">
-        <f>RANK(J24,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="L24">
@@ -3872,15 +3862,15 @@
         <v>1112527.1200000001</v>
       </c>
       <c r="N24">
-        <f>M24-L24</f>
+        <f t="shared" si="5"/>
         <v>-72.879999999888241</v>
       </c>
       <c r="O24" s="5">
-        <f>IFERROR(N24/L24, 0)</f>
+        <f t="shared" si="6"/>
         <v>-6.5504224339284781E-5</v>
       </c>
       <c r="P24">
-        <f>RANK(O24,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>41</v>
       </c>
     </row>
@@ -3895,15 +3885,15 @@
         <v>479149.53</v>
       </c>
       <c r="D25">
-        <f>C25-B25</f>
+        <f t="shared" si="0"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="E25" s="5">
-        <f>IFERROR(D25/B25, 0)</f>
+        <f t="shared" si="1"/>
         <v>-1.0226130964676661E-2</v>
       </c>
       <c r="F25">
-        <f>RANK(E25,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>38</v>
       </c>
       <c r="G25">
@@ -3913,15 +3903,15 @@
         <v>497194.20999999897</v>
       </c>
       <c r="I25">
-        <f>H25-G25</f>
+        <f t="shared" si="2"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="J25" s="5">
-        <f>IFERROR(I25/G25, 0)</f>
+        <f t="shared" si="3"/>
         <v>-1.5846773555029746E-2</v>
       </c>
       <c r="K25">
-        <f>RANK(J25,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="L25">
@@ -3931,15 +3921,15 @@
         <v>494775.1</v>
       </c>
       <c r="N25">
-        <f>M25-L25</f>
+        <f t="shared" si="5"/>
         <v>-1724.9000000000233</v>
       </c>
       <c r="O25" s="5">
-        <f>IFERROR(N25/L25, 0)</f>
+        <f t="shared" si="6"/>
         <v>-3.4741188318228064E-3</v>
       </c>
       <c r="P25">
-        <f>RANK(O25,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
     </row>
@@ -3954,15 +3944,15 @@
         <v>4801960.08</v>
       </c>
       <c r="D26">
-        <f>C26-B26</f>
+        <f t="shared" si="0"/>
         <v>-447839.91999999993</v>
       </c>
       <c r="E26" s="5">
-        <f>IFERROR(D26/B26, 0)</f>
+        <f t="shared" si="1"/>
         <v>-8.5306091660634673E-2</v>
       </c>
       <c r="F26">
-        <f>RANK(E26,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="G26">
@@ -3972,15 +3962,15 @@
         <v>5122329.02999999</v>
       </c>
       <c r="I26">
-        <f>H26-G26</f>
+        <f t="shared" si="2"/>
         <v>-319870.97000000998</v>
       </c>
       <c r="J26" s="5">
-        <f>IFERROR(I26/G26, 0)</f>
+        <f t="shared" si="3"/>
         <v>-5.8776040939327839E-2</v>
       </c>
       <c r="K26">
-        <f>RANK(J26,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="L26">
@@ -3990,15 +3980,15 @@
         <v>5117235.21</v>
       </c>
       <c r="N26">
-        <f>M26-L26</f>
+        <f t="shared" si="5"/>
         <v>-313464.79000000004</v>
       </c>
       <c r="O26" s="5">
-        <f>IFERROR(N26/L26, 0)</f>
+        <f t="shared" si="6"/>
         <v>-5.7720881286022069E-2</v>
       </c>
       <c r="P26">
-        <f>RANK(O26,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
     </row>
@@ -4013,15 +4003,15 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <f>C27-B27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E27" s="5">
-        <f>IFERROR(D27/B27, 0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F27">
-        <f>RANK(E27,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>47</v>
       </c>
       <c r="G27">
@@ -4031,15 +4021,15 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <f>H27-G27</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J27" s="5">
-        <f>IFERROR(I27/G27, 0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K27">
-        <f>RANK(J27,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="L27">
@@ -4049,15 +4039,15 @@
         <v>0</v>
       </c>
       <c r="N27">
-        <f>M27-L27</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O27" s="5">
-        <f>IFERROR(N27/L27, 0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P27">
-        <f>RANK(O27,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
     </row>
@@ -4072,15 +4062,15 @@
         <v>1250442.02</v>
       </c>
       <c r="D28">
-        <f>C28-B28</f>
+        <f t="shared" si="0"/>
         <v>-132457.97999999998</v>
       </c>
       <c r="E28" s="5">
-        <f>IFERROR(D28/B28, 0)</f>
+        <f t="shared" si="1"/>
         <v>-9.5782760864849215E-2</v>
       </c>
       <c r="F28">
-        <f>RANK(E28,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="G28">
@@ -4090,15 +4080,15 @@
         <v>1281335.23</v>
       </c>
       <c r="I28">
-        <f>H28-G28</f>
+        <f t="shared" si="2"/>
         <v>-264364.77</v>
       </c>
       <c r="J28" s="5">
-        <f>IFERROR(I28/G28, 0)</f>
+        <f t="shared" si="3"/>
         <v>-0.17103239309050916</v>
       </c>
       <c r="K28">
-        <f>RANK(J28,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L28">
@@ -4108,15 +4098,15 @@
         <v>1393285.06</v>
       </c>
       <c r="N28">
-        <f>M28-L28</f>
+        <f t="shared" si="5"/>
         <v>-132614.93999999994</v>
       </c>
       <c r="O28" s="5">
-        <f>IFERROR(N28/L28, 0)</f>
+        <f t="shared" si="6"/>
         <v>-8.6909325643882263E-2</v>
       </c>
       <c r="P28">
-        <f>RANK(O28,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4131,15 +4121,15 @@
         <v>2523884.71</v>
       </c>
       <c r="D29">
-        <f>C29-B29</f>
+        <f t="shared" si="0"/>
         <v>-37915.290000000037</v>
       </c>
       <c r="E29" s="5">
-        <f>IFERROR(D29/B29, 0)</f>
+        <f t="shared" si="1"/>
         <v>-1.4800253727847622E-2</v>
       </c>
       <c r="F29">
-        <f>RANK(E29,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
       <c r="G29">
@@ -4149,15 +4139,15 @@
         <v>2665264.4399999902</v>
       </c>
       <c r="I29">
-        <f>H29-G29</f>
+        <f t="shared" si="2"/>
         <v>-114235.56000000983</v>
       </c>
       <c r="J29" s="5">
-        <f>IFERROR(I29/G29, 0)</f>
+        <f t="shared" si="3"/>
         <v>-4.1099320021590155E-2</v>
       </c>
       <c r="K29">
-        <f>RANK(J29,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="L29">
@@ -4167,15 +4157,15 @@
         <v>2889864.67</v>
       </c>
       <c r="N29">
-        <f>M29-L29</f>
+        <f t="shared" si="5"/>
         <v>-35.330000000074506</v>
       </c>
       <c r="O29" s="5">
-        <f>IFERROR(N29/L29, 0)</f>
+        <f t="shared" si="6"/>
         <v>-1.2225336516860273E-5</v>
       </c>
       <c r="P29">
-        <f>RANK(O29,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
     </row>
@@ -4190,15 +4180,15 @@
         <v>12030494.1</v>
       </c>
       <c r="D30">
-        <f>C30-B30</f>
+        <f t="shared" si="0"/>
         <v>-101705.90000000037</v>
       </c>
       <c r="E30" s="5">
-        <f>IFERROR(D30/B30, 0)</f>
+        <f t="shared" si="1"/>
         <v>-8.3831374359143746E-3</v>
       </c>
       <c r="F30">
-        <f>RANK(E30,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="G30">
@@ -4208,15 +4198,15 @@
         <v>12685514.279999901</v>
       </c>
       <c r="I30">
-        <f>H30-G30</f>
+        <f t="shared" si="2"/>
         <v>-50385.720000099391</v>
       </c>
       <c r="J30" s="5">
-        <f>IFERROR(I30/G30, 0)</f>
+        <f t="shared" si="3"/>
         <v>-3.9561962641116366E-3</v>
       </c>
       <c r="K30">
-        <f>RANK(J30,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="L30">
@@ -4226,15 +4216,15 @@
         <v>12826009.609999999</v>
       </c>
       <c r="N30">
-        <f>M30-L30</f>
+        <f t="shared" si="5"/>
         <v>-35290.390000000596</v>
       </c>
       <c r="O30" s="5">
-        <f>IFERROR(N30/L30, 0)</f>
+        <f t="shared" si="6"/>
         <v>-2.7439209100169185E-3</v>
       </c>
       <c r="P30">
-        <f>RANK(O30,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
     </row>
@@ -4249,15 +4239,15 @@
         <v>1740827.69</v>
       </c>
       <c r="D31">
-        <f>C31-B31</f>
+        <f t="shared" si="0"/>
         <v>-24772.310000000056</v>
       </c>
       <c r="E31" s="5">
-        <f>IFERROR(D31/B31, 0)</f>
+        <f t="shared" si="1"/>
         <v>-1.4030533529678329E-2</v>
       </c>
       <c r="F31">
-        <f>RANK(E31,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="G31">
@@ -4267,15 +4257,15 @@
         <v>1762676.85</v>
       </c>
       <c r="I31">
-        <f>H31-G31</f>
+        <f t="shared" si="2"/>
         <v>-60623.149999999907</v>
       </c>
       <c r="J31" s="5">
-        <f>IFERROR(I31/G31, 0)</f>
+        <f t="shared" si="3"/>
         <v>-3.3249136181648611E-2</v>
       </c>
       <c r="K31">
-        <f>RANK(J31,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="L31">
@@ -4285,15 +4275,15 @@
         <v>1801391.34</v>
       </c>
       <c r="N31">
-        <f>M31-L31</f>
+        <f t="shared" si="5"/>
         <v>-69308.659999999916</v>
       </c>
       <c r="O31" s="5">
-        <f>IFERROR(N31/L31, 0)</f>
+        <f t="shared" si="6"/>
         <v>-3.7049585716576634E-2</v>
       </c>
       <c r="P31">
-        <f>RANK(O31,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
     </row>
@@ -4308,15 +4298,15 @@
         <v>5925637.7199999904</v>
       </c>
       <c r="D32">
-        <f>C32-B32</f>
+        <f t="shared" si="0"/>
         <v>-73762.280000009574</v>
       </c>
       <c r="E32" s="5">
-        <f>IFERROR(D32/B32, 0)</f>
+        <f t="shared" si="1"/>
         <v>-1.2294942827617691E-2</v>
       </c>
       <c r="F32">
-        <f>RANK(E32,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
       <c r="G32">
@@ -4326,15 +4316,15 @@
         <v>6084985.4699999997</v>
       </c>
       <c r="I32">
-        <f>H32-G32</f>
+        <f t="shared" si="2"/>
         <v>-110514.53000000026</v>
       </c>
       <c r="J32" s="5">
-        <f>IFERROR(I32/G32, 0)</f>
+        <f t="shared" si="3"/>
         <v>-1.7837871035428981E-2</v>
       </c>
       <c r="K32">
-        <f>RANK(J32,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="L32">
@@ -4344,15 +4334,15 @@
         <v>5987572.0199999996</v>
       </c>
       <c r="N32">
-        <f>M32-L32</f>
+        <f t="shared" si="5"/>
         <v>-169827.98000000045</v>
       </c>
       <c r="O32" s="5">
-        <f>IFERROR(N32/L32, 0)</f>
+        <f t="shared" si="6"/>
         <v>-2.7581118653977402E-2</v>
       </c>
       <c r="P32">
-        <f>RANK(O32,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
     </row>
@@ -4367,15 +4357,15 @@
         <v>920284264.73000002</v>
       </c>
       <c r="D33">
-        <f>C33-B33</f>
+        <f t="shared" si="0"/>
         <v>-7418835.2699990273</v>
       </c>
       <c r="E33" s="5">
-        <f>IFERROR(D33/B33, 0)</f>
+        <f t="shared" si="1"/>
         <v>-7.9969930789269058E-3</v>
       </c>
       <c r="F33">
-        <f>RANK(E33,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>41</v>
       </c>
       <c r="G33">
@@ -4385,15 +4375,15 @@
         <v>977068513.48000002</v>
       </c>
       <c r="I33">
-        <f>H33-G33</f>
+        <f t="shared" si="2"/>
         <v>-2602486.5199999809</v>
       </c>
       <c r="J33" s="5">
-        <f>IFERROR(I33/G33, 0)</f>
+        <f t="shared" si="3"/>
         <v>-2.6564903115433454E-3</v>
       </c>
       <c r="K33">
-        <f>RANK(J33,J:J,1)</f>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="L33">
@@ -4403,15 +4393,15 @@
         <v>984116289.40999901</v>
       </c>
       <c r="N33">
-        <f>M33-L33</f>
+        <f t="shared" si="5"/>
         <v>-5456610.5900000334</v>
       </c>
       <c r="O33" s="5">
-        <f>IFERROR(N33/L33, 0)</f>
+        <f t="shared" si="6"/>
         <v>-5.5141067323084929E-3</v>
       </c>
       <c r="P33">
-        <f>RANK(O33,O:O,1)</f>
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
     </row>
@@ -4426,15 +4416,15 @@
         <v>4109958.22</v>
       </c>
       <c r="D34">
-        <f>C34-B34</f>
+        <f t="shared" ref="D34:D65" si="9">C34-B34</f>
         <v>-79341.779999999795</v>
       </c>
       <c r="E34" s="5">
-        <f>IFERROR(D34/B34, 0)</f>
+        <f t="shared" ref="E34:E52" si="10">IFERROR(D34/B34, 0)</f>
         <v>-1.8939149738619768E-2</v>
       </c>
       <c r="F34">
-        <f>RANK(E34,E:E,1)</f>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="G34">
@@ -4444,15 +4434,15 @@
         <v>4137588.7699999898</v>
       </c>
       <c r="I34">
-        <f>H34-G34</f>
+        <f t="shared" ref="I34:I65" si="11">H34-G34</f>
         <v>-213011.23000001023</v>
       </c>
       <c r="J34" s="5">
-        <f>IFERROR(I34/G34, 0)</f>
+        <f t="shared" ref="J34:J52" si="12">IFERROR(I34/G34, 0)</f>
         <v>-4.8961345561534093E-2</v>
       </c>
       <c r="K34">
-        <f>RANK(J34,J:J,1)</f>
+        <f t="shared" ref="K34:K52" si="13">RANK(J34,J:J,1)</f>
         <v>21</v>
       </c>
       <c r="L34">
@@ -4462,15 +4452,15 @@
         <v>4229801.51</v>
       </c>
       <c r="N34">
-        <f>M34-L34</f>
+        <f t="shared" ref="N34:N65" si="14">M34-L34</f>
         <v>-115798.49000000022</v>
       </c>
       <c r="O34" s="5">
-        <f>IFERROR(N34/L34, 0)</f>
+        <f t="shared" ref="O34:O52" si="15">IFERROR(N34/L34, 0)</f>
         <v>-2.6647296115611244E-2</v>
       </c>
       <c r="P34">
-        <f>RANK(O34,O:O,1)</f>
+        <f t="shared" ref="P34:P52" si="16">RANK(O34,O:O,1)</f>
         <v>24</v>
       </c>
     </row>
@@ -4485,15 +4475,15 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <f>C35-B35</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E35" s="5">
-        <f>IFERROR(D35/B35, 0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F35">
-        <f>RANK(E35,E:E,1)</f>
+        <f t="shared" ref="F35:F52" si="17">RANK(E35,E:E,1)</f>
         <v>47</v>
       </c>
       <c r="G35">
@@ -4503,15 +4493,15 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <f>H35-G35</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J35" s="5">
-        <f>IFERROR(I35/G35, 0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K35">
-        <f>RANK(J35,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>48</v>
       </c>
       <c r="L35">
@@ -4521,15 +4511,15 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <f>M35-L35</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O35" s="5">
-        <f>IFERROR(N35/L35, 0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P35">
-        <f>RANK(O35,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>48</v>
       </c>
     </row>
@@ -4544,15 +4534,15 @@
         <v>735423.27999999898</v>
       </c>
       <c r="D36">
-        <f>C36-B36</f>
+        <f t="shared" si="9"/>
         <v>-62776.72000000102</v>
       </c>
       <c r="E36" s="5">
-        <f>IFERROR(D36/B36, 0)</f>
+        <f t="shared" si="10"/>
         <v>-7.8647857679780775E-2</v>
       </c>
       <c r="F36">
-        <f>RANK(E36,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
       <c r="G36">
@@ -4562,15 +4552,15 @@
         <v>740966.94999999902</v>
       </c>
       <c r="I36">
-        <f>H36-G36</f>
+        <f t="shared" si="11"/>
         <v>-157733.05000000098</v>
       </c>
       <c r="J36" s="5">
-        <f>IFERROR(I36/G36, 0)</f>
+        <f t="shared" si="12"/>
         <v>-0.17551246244575608</v>
       </c>
       <c r="K36">
-        <f>RANK(J36,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L36">
@@ -4580,15 +4570,15 @@
         <v>777215.28999999899</v>
       </c>
       <c r="N36">
-        <f>M36-L36</f>
+        <f t="shared" si="14"/>
         <v>-101084.71000000101</v>
       </c>
       <c r="O36" s="5">
-        <f>IFERROR(N36/L36, 0)</f>
+        <f t="shared" si="15"/>
         <v>-0.11509132414892521</v>
       </c>
       <c r="P36">
-        <f>RANK(O36,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
     </row>
@@ -4603,15 +4593,15 @@
         <v>2005447.73999999</v>
       </c>
       <c r="D37">
-        <f>C37-B37</f>
+        <f t="shared" si="9"/>
         <v>-82352.260000010021</v>
       </c>
       <c r="E37" s="5">
-        <f>IFERROR(D37/B37, 0)</f>
+        <f t="shared" si="10"/>
         <v>-3.9444515758219188E-2</v>
       </c>
       <c r="F37">
-        <f>RANK(E37,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>19</v>
       </c>
       <c r="G37">
@@ -4621,15 +4611,15 @@
         <v>2118943.21</v>
       </c>
       <c r="I37">
-        <f>H37-G37</f>
+        <f t="shared" si="11"/>
         <v>-110256.79000000004</v>
       </c>
       <c r="J37" s="5">
-        <f>IFERROR(I37/G37, 0)</f>
+        <f t="shared" si="12"/>
         <v>-4.9460250314014013E-2</v>
       </c>
       <c r="K37">
-        <f>RANK(J37,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
       <c r="L37">
@@ -4639,15 +4629,15 @@
         <v>2108718.34</v>
       </c>
       <c r="N37">
-        <f>M37-L37</f>
+        <f t="shared" si="14"/>
         <v>-188181.66000000015</v>
       </c>
       <c r="O37" s="5">
-        <f>IFERROR(N37/L37, 0)</f>
+        <f t="shared" si="15"/>
         <v>-8.1928538464887526E-2</v>
       </c>
       <c r="P37">
-        <f>RANK(O37,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
     </row>
@@ -4662,15 +4652,15 @@
         <v>838669.82</v>
       </c>
       <c r="D38">
-        <f>C38-B38</f>
+        <f t="shared" si="9"/>
         <v>-16630.180000000051</v>
       </c>
       <c r="E38" s="5">
-        <f>IFERROR(D38/B38, 0)</f>
+        <f t="shared" si="10"/>
         <v>-1.9443680579913542E-2</v>
       </c>
       <c r="F38">
-        <f>RANK(E38,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>25</v>
       </c>
       <c r="G38">
@@ -4680,15 +4670,15 @@
         <v>753451.96</v>
       </c>
       <c r="I38">
-        <f>H38-G38</f>
+        <f t="shared" si="11"/>
         <v>-39348.040000000037</v>
       </c>
       <c r="J38" s="5">
-        <f>IFERROR(I38/G38, 0)</f>
+        <f t="shared" si="12"/>
         <v>-4.9631735620585316E-2</v>
       </c>
       <c r="K38">
-        <f>RANK(J38,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>19</v>
       </c>
       <c r="L38">
@@ -4698,15 +4688,15 @@
         <v>777663.26</v>
       </c>
       <c r="N38">
-        <f>M38-L38</f>
+        <f t="shared" si="14"/>
         <v>-136.73999999999069</v>
       </c>
       <c r="O38" s="5">
-        <f>IFERROR(N38/L38, 0)</f>
+        <f t="shared" si="15"/>
         <v>-1.7580354847003174E-4</v>
       </c>
       <c r="P38">
-        <f>RANK(O38,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>40</v>
       </c>
     </row>
@@ -4721,15 +4711,15 @@
         <v>813108.87</v>
       </c>
       <c r="D39">
-        <f>C39-B39</f>
+        <f t="shared" si="9"/>
         <v>-70791.13</v>
       </c>
       <c r="E39" s="5">
-        <f>IFERROR(D39/B39, 0)</f>
+        <f t="shared" si="10"/>
         <v>-8.008952370177623E-2</v>
       </c>
       <c r="F39">
-        <f>RANK(E39,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="G39">
@@ -4739,15 +4729,15 @@
         <v>1114242.27999999</v>
       </c>
       <c r="I39">
-        <f>H39-G39</f>
+        <f t="shared" si="11"/>
         <v>-180157.72000000998</v>
       </c>
       <c r="J39" s="5">
-        <f>IFERROR(I39/G39, 0)</f>
+        <f t="shared" si="12"/>
         <v>-0.13918241656366656</v>
       </c>
       <c r="K39">
-        <f>RANK(J39,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="L39">
@@ -4757,15 +4747,15 @@
         <v>1680463.8699999901</v>
       </c>
       <c r="N39">
-        <f>M39-L39</f>
+        <f t="shared" si="14"/>
         <v>-79036.1300000099</v>
       </c>
       <c r="O39" s="5">
-        <f>IFERROR(N39/L39, 0)</f>
+        <f t="shared" si="15"/>
         <v>-4.4919653310605226E-2</v>
       </c>
       <c r="P39">
-        <f>RANK(O39,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>17</v>
       </c>
     </row>
@@ -4780,15 +4770,15 @@
         <v>37565141.859999903</v>
       </c>
       <c r="D40">
-        <f>C40-B40</f>
+        <f t="shared" si="9"/>
         <v>-816758.14000009745</v>
       </c>
       <c r="E40" s="5">
-        <f>IFERROR(D40/B40, 0)</f>
+        <f t="shared" si="10"/>
         <v>-2.1279773539092578E-2</v>
       </c>
       <c r="F40">
-        <f>RANK(E40,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>23</v>
       </c>
       <c r="G40">
@@ -4798,15 +4788,15 @@
         <v>38095240.189999901</v>
       </c>
       <c r="I40">
-        <f>H40-G40</f>
+        <f t="shared" si="11"/>
         <v>-1869659.8100000992</v>
       </c>
       <c r="J40" s="5">
-        <f>IFERROR(I40/G40, 0)</f>
+        <f t="shared" si="12"/>
         <v>-4.6782546934937892E-2</v>
       </c>
       <c r="K40">
-        <f>RANK(J40,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="L40">
@@ -4816,15 +4806,15 @@
         <v>39606263.709999897</v>
       </c>
       <c r="N40">
-        <f>M40-L40</f>
+        <f t="shared" si="14"/>
         <v>-610436.29000010341</v>
       </c>
       <c r="O40" s="5">
-        <f>IFERROR(N40/L40, 0)</f>
+        <f t="shared" si="15"/>
         <v>-1.5178676768608648E-2</v>
       </c>
       <c r="P40">
-        <f>RANK(O40,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
     </row>
@@ -4839,15 +4829,15 @@
         <v>4409060.2099999897</v>
       </c>
       <c r="D41">
-        <f>C41-B41</f>
+        <f t="shared" si="9"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="E41" s="5">
-        <f>IFERROR(D41/B41, 0)</f>
+        <f t="shared" si="10"/>
         <v>-4.0110550149132493E-2</v>
       </c>
       <c r="F41">
-        <f>RANK(E41,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>17</v>
       </c>
       <c r="G41">
@@ -4857,15 +4847,15 @@
         <v>4956043.6699999897</v>
       </c>
       <c r="I41">
-        <f>H41-G41</f>
+        <f t="shared" si="11"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="J41" s="5">
-        <f>IFERROR(I41/G41, 0)</f>
+        <f t="shared" si="12"/>
         <v>-2.6221894095689226E-2</v>
       </c>
       <c r="K41">
-        <f>RANK(J41,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>34</v>
       </c>
       <c r="L41">
@@ -4875,15 +4865,15 @@
         <v>4717822.6500000004</v>
       </c>
       <c r="N41">
-        <f>M41-L41</f>
+        <f t="shared" si="14"/>
         <v>-82077.349999999627</v>
       </c>
       <c r="O41" s="5">
-        <f>IFERROR(N41/L41, 0)</f>
+        <f t="shared" si="15"/>
         <v>-1.7099804162586642E-2</v>
       </c>
       <c r="P41">
-        <f>RANK(O41,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>30</v>
       </c>
     </row>
@@ -4898,15 +4888,15 @@
         <v>188551675.67999899</v>
       </c>
       <c r="D42">
-        <f>C42-B42</f>
+        <f t="shared" si="9"/>
         <v>-41624.320001006126</v>
       </c>
       <c r="E42" s="5">
-        <f>IFERROR(D42/B42, 0)</f>
+        <f t="shared" si="10"/>
         <v>-2.2070943135841053E-4</v>
       </c>
       <c r="F42">
-        <f>RANK(E42,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>44</v>
       </c>
       <c r="G42">
@@ -4916,15 +4906,15 @@
         <v>196755033.31</v>
       </c>
       <c r="I42">
-        <f>H42-G42</f>
+        <f t="shared" si="11"/>
         <v>-2375266.6899999976</v>
       </c>
       <c r="J42" s="5">
-        <f>IFERROR(I42/G42, 0)</f>
+        <f t="shared" si="12"/>
         <v>-1.1928203241796942E-2</v>
       </c>
       <c r="K42">
-        <f>RANK(J42,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>39</v>
       </c>
       <c r="L42">
@@ -4934,15 +4924,15 @@
         <v>199954563.74999899</v>
       </c>
       <c r="N42">
-        <f>M42-L42</f>
+        <f t="shared" si="14"/>
         <v>-36.250001013278961</v>
       </c>
       <c r="O42" s="5">
-        <f>IFERROR(N42/L42, 0)</f>
+        <f t="shared" si="15"/>
         <v>-1.8129115815929696E-7</v>
       </c>
       <c r="P42">
-        <f>RANK(O42,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>47</v>
       </c>
     </row>
@@ -4957,15 +4947,15 @@
         <v>7968645.8300000001</v>
       </c>
       <c r="D43">
-        <f>C43-B43</f>
+        <f t="shared" si="9"/>
         <v>-166754.16999999993</v>
       </c>
       <c r="E43" s="5">
-        <f>IFERROR(D43/B43, 0)</f>
+        <f t="shared" si="10"/>
         <v>-2.0497353541313264E-2</v>
       </c>
       <c r="F43">
-        <f>RANK(E43,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>24</v>
       </c>
       <c r="G43">
@@ -4975,15 +4965,15 @@
         <v>8171472.0199999996</v>
       </c>
       <c r="I43">
-        <f>H43-G43</f>
+        <f t="shared" si="11"/>
         <v>-389327.98000000045</v>
       </c>
       <c r="J43" s="5">
-        <f>IFERROR(I43/G43, 0)</f>
+        <f t="shared" si="12"/>
         <v>-4.5477990374731388E-2</v>
       </c>
       <c r="K43">
-        <f>RANK(J43,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="L43">
@@ -4993,15 +4983,15 @@
         <v>8150982.5699999901</v>
       </c>
       <c r="N43">
-        <f>M43-L43</f>
+        <f t="shared" si="14"/>
         <v>-346517.43000000995</v>
       </c>
       <c r="O43" s="5">
-        <f>IFERROR(N43/L43, 0)</f>
+        <f t="shared" si="15"/>
         <v>-4.0778750220654303E-2</v>
       </c>
       <c r="P43">
-        <f>RANK(O43,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>18</v>
       </c>
     </row>
@@ -5016,15 +5006,15 @@
         <v>29789104.379999999</v>
       </c>
       <c r="D44">
-        <f>C44-B44</f>
+        <f t="shared" si="9"/>
         <v>-294095.62000000104</v>
       </c>
       <c r="E44" s="5">
-        <f>IFERROR(D44/B44, 0)</f>
+        <f t="shared" si="10"/>
         <v>-9.7760750186150751E-3</v>
       </c>
       <c r="F44">
-        <f>RANK(E44,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>39</v>
       </c>
       <c r="G44">
@@ -5034,15 +5024,15 @@
         <v>30793711.48</v>
       </c>
       <c r="I44">
-        <f>H44-G44</f>
+        <f t="shared" si="11"/>
         <v>-246988.51999999955</v>
       </c>
       <c r="J44" s="5">
-        <f>IFERROR(I44/G44, 0)</f>
+        <f t="shared" si="12"/>
         <v>-7.9569249404813532E-3</v>
       </c>
       <c r="K44">
-        <f>RANK(J44,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>41</v>
       </c>
       <c r="L44">
@@ -5052,15 +5042,15 @@
         <v>31282141.25</v>
       </c>
       <c r="N44">
-        <f>M44-L44</f>
+        <f t="shared" si="14"/>
         <v>-58.75</v>
       </c>
       <c r="O44" s="5">
-        <f>IFERROR(N44/L44, 0)</f>
+        <f t="shared" si="15"/>
         <v>-1.8780648419868168E-6</v>
       </c>
       <c r="P44">
-        <f>RANK(O44,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>45</v>
       </c>
     </row>
@@ -5075,15 +5065,15 @@
         <v>54589584.0499999</v>
       </c>
       <c r="D45">
-        <f>C45-B45</f>
+        <f t="shared" si="9"/>
         <v>-712015.95000009984</v>
       </c>
       <c r="E45" s="5">
-        <f>IFERROR(D45/B45, 0)</f>
+        <f t="shared" si="10"/>
         <v>-1.287514194887851E-2</v>
       </c>
       <c r="F45">
-        <f>RANK(E45,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>34</v>
       </c>
       <c r="G45">
@@ -5093,15 +5083,15 @@
         <v>54594953.959999897</v>
       </c>
       <c r="I45">
-        <f>H45-G45</f>
+        <f t="shared" si="11"/>
         <v>-2197246.0400001034</v>
       </c>
       <c r="J45" s="5">
-        <f>IFERROR(I45/G45, 0)</f>
+        <f t="shared" si="12"/>
         <v>-3.8689222111488959E-2</v>
       </c>
       <c r="K45">
-        <f>RANK(J45,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
       <c r="L45">
@@ -5111,15 +5101,15 @@
         <v>55386549.6599999</v>
       </c>
       <c r="N45">
-        <f>M45-L45</f>
+        <f t="shared" si="14"/>
         <v>-640550.34000010043</v>
       </c>
       <c r="O45" s="5">
-        <f>IFERROR(N45/L45, 0)</f>
+        <f t="shared" si="15"/>
         <v>-1.1432866237947358E-2</v>
       </c>
       <c r="P45">
-        <f>RANK(O45,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>32</v>
       </c>
     </row>
@@ -5134,15 +5124,15 @@
         <v>258322.43</v>
       </c>
       <c r="D46">
-        <f>C46-B46</f>
+        <f t="shared" si="9"/>
         <v>-777.57000000000698</v>
       </c>
       <c r="E46" s="5">
-        <f>IFERROR(D46/B46, 0)</f>
+        <f t="shared" si="10"/>
         <v>-3.0010420686993711E-3</v>
       </c>
       <c r="F46">
-        <f>RANK(E46,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>43</v>
       </c>
       <c r="G46">
@@ -5152,15 +5142,15 @@
         <v>257402.90999999901</v>
       </c>
       <c r="I46">
-        <f>H46-G46</f>
+        <f t="shared" si="11"/>
         <v>-8597.090000000986</v>
       </c>
       <c r="J46" s="5">
-        <f>IFERROR(I46/G46, 0)</f>
+        <f t="shared" si="12"/>
         <v>-3.2319887218048821E-2</v>
       </c>
       <c r="K46">
-        <f>RANK(J46,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>33</v>
       </c>
       <c r="L46">
@@ -5170,15 +5160,15 @@
         <v>254753.15999999901</v>
       </c>
       <c r="N46">
-        <f>M46-L46</f>
+        <f t="shared" si="14"/>
         <v>-12346.840000000986</v>
       </c>
       <c r="O46" s="5">
-        <f>IFERROR(N46/L46, 0)</f>
+        <f t="shared" si="15"/>
         <v>-4.6225533508053113E-2</v>
       </c>
       <c r="P46">
-        <f>RANK(O46,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>16</v>
       </c>
     </row>
@@ -5193,15 +5183,15 @@
         <v>70378426.719999999</v>
       </c>
       <c r="D47">
-        <f>C47-B47</f>
+        <f t="shared" si="9"/>
         <v>-12273.280000001192</v>
       </c>
       <c r="E47" s="5">
-        <f>IFERROR(D47/B47, 0)</f>
+        <f t="shared" si="10"/>
         <v>-1.7435939690898361E-4</v>
       </c>
       <c r="F47">
-        <f>RANK(E47,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>45</v>
       </c>
       <c r="G47">
@@ -5211,15 +5201,15 @@
         <v>73442541.659999996</v>
       </c>
       <c r="I47">
-        <f>H47-G47</f>
+        <f t="shared" si="11"/>
         <v>-24458.340000003576</v>
       </c>
       <c r="J47" s="5">
-        <f>IFERROR(I47/G47, 0)</f>
+        <f t="shared" si="12"/>
         <v>-3.3291600310348285E-4</v>
       </c>
       <c r="K47">
-        <f>RANK(J47,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="L47">
@@ -5229,15 +5219,15 @@
         <v>75050829.179999903</v>
       </c>
       <c r="N47">
-        <f>M47-L47</f>
+        <f t="shared" si="14"/>
         <v>-21970.820000097156</v>
       </c>
       <c r="O47" s="5">
-        <f>IFERROR(N47/L47, 0)</f>
+        <f t="shared" si="15"/>
         <v>-2.9266019117572752E-4</v>
       </c>
       <c r="P47">
-        <f>RANK(O47,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>38</v>
       </c>
     </row>
@@ -5252,15 +5242,15 @@
         <v>6527352.5699999901</v>
       </c>
       <c r="D48">
-        <f>C48-B48</f>
+        <f t="shared" si="9"/>
         <v>-209747.43000000995</v>
       </c>
       <c r="E48" s="5">
-        <f>IFERROR(D48/B48, 0)</f>
+        <f t="shared" si="10"/>
         <v>-3.1133192323107857E-2</v>
       </c>
       <c r="F48">
-        <f>RANK(E48,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="G48">
@@ -5270,15 +5260,15 @@
         <v>6922072.5599999996</v>
       </c>
       <c r="I48">
-        <f>H48-G48</f>
+        <f t="shared" si="11"/>
         <v>-292627.44000000041</v>
       </c>
       <c r="J48" s="5">
-        <f>IFERROR(I48/G48, 0)</f>
+        <f t="shared" si="12"/>
         <v>-4.0559890224125802E-2</v>
       </c>
       <c r="K48">
-        <f>RANK(J48,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="L48">
@@ -5288,15 +5278,15 @@
         <v>6882350.23999999</v>
       </c>
       <c r="N48">
-        <f>M48-L48</f>
+        <f t="shared" si="14"/>
         <v>-407449.76000001002</v>
       </c>
       <c r="O48" s="5">
-        <f>IFERROR(N48/L48, 0)</f>
+        <f t="shared" si="15"/>
         <v>-5.5893132870587676E-2</v>
       </c>
       <c r="P48">
-        <f>RANK(O48,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>15</v>
       </c>
     </row>
@@ -5311,15 +5301,15 @@
         <v>90499.43</v>
       </c>
       <c r="D49">
-        <f>C49-B49</f>
+        <f t="shared" si="9"/>
         <v>-1700.570000000007</v>
       </c>
       <c r="E49" s="5">
-        <f>IFERROR(D49/B49, 0)</f>
+        <f t="shared" si="10"/>
         <v>-1.8444360086767971E-2</v>
       </c>
       <c r="F49">
-        <f>RANK(E49,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>27</v>
       </c>
       <c r="G49">
@@ -5329,15 +5319,15 @@
         <v>95466.880000000005</v>
       </c>
       <c r="I49">
-        <f>H49-G49</f>
+        <f t="shared" si="11"/>
         <v>-7133.1199999999953</v>
       </c>
       <c r="J49" s="5">
-        <f>IFERROR(I49/G49, 0)</f>
+        <f t="shared" si="12"/>
         <v>-6.9523586744639335E-2</v>
       </c>
       <c r="K49">
-        <f>RANK(J49,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>13</v>
       </c>
       <c r="L49">
@@ -5347,15 +5337,15 @@
         <v>0</v>
       </c>
       <c r="N49">
-        <f>M49-L49</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O49" s="5">
-        <f>IFERROR(N49/L49, 0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P49">
-        <f>RANK(O49,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>48</v>
       </c>
     </row>
@@ -5370,15 +5360,15 @@
         <v>832600</v>
       </c>
       <c r="D50">
-        <f>C50-B50</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E50" s="5">
-        <f>IFERROR(D50/B50, 0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F50">
-        <f>RANK(E50,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>47</v>
       </c>
       <c r="G50">
@@ -5388,15 +5378,15 @@
         <v>859100</v>
       </c>
       <c r="I50">
-        <f>H50-G50</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J50" s="5">
-        <f>IFERROR(I50/G50, 0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K50">
-        <f>RANK(J50,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>48</v>
       </c>
       <c r="L50">
@@ -5406,15 +5396,15 @@
         <v>843200</v>
       </c>
       <c r="N50">
-        <f>M50-L50</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O50" s="5">
-        <f>IFERROR(N50/L50, 0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P50">
-        <f>RANK(O50,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>48</v>
       </c>
     </row>
@@ -5429,15 +5419,15 @@
         <v>8499425.3399999905</v>
       </c>
       <c r="D51">
-        <f>C51-B51</f>
+        <f t="shared" si="9"/>
         <v>-110074.66000000946</v>
       </c>
       <c r="E51" s="5">
-        <f>IFERROR(D51/B51, 0)</f>
+        <f t="shared" si="10"/>
         <v>-1.2785255822058129E-2</v>
       </c>
       <c r="F51">
-        <f>RANK(E51,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>35</v>
       </c>
       <c r="G51">
@@ -5447,15 +5437,15 @@
         <v>8599059.6199999992</v>
       </c>
       <c r="I51">
-        <f>H51-G51</f>
+        <f t="shared" si="11"/>
         <v>-326440.38000000082</v>
       </c>
       <c r="J51" s="5">
-        <f>IFERROR(I51/G51, 0)</f>
+        <f t="shared" si="12"/>
         <v>-3.6573903982970231E-2</v>
       </c>
       <c r="K51">
-        <f>RANK(J51,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>31</v>
       </c>
       <c r="L51">
@@ -5465,15 +5455,15 @@
         <v>8735843.3100000005</v>
       </c>
       <c r="N51">
-        <f>M51-L51</f>
+        <f t="shared" si="14"/>
         <v>-98056.689999999478</v>
       </c>
       <c r="O51" s="5">
-        <f>IFERROR(N51/L51, 0)</f>
+        <f t="shared" si="15"/>
         <v>-1.1100045280114048E-2</v>
       </c>
       <c r="P51">
-        <f>RANK(O51,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>33</v>
       </c>
     </row>
@@ -5488,15 +5478,15 @@
         <v>2254684.7999999998</v>
       </c>
       <c r="D52">
-        <f>C52-B52</f>
+        <f t="shared" si="9"/>
         <v>-196315.20000000019</v>
       </c>
       <c r="E52" s="5">
-        <f>IFERROR(D52/B52, 0)</f>
+        <f t="shared" si="10"/>
         <v>-8.009596083231342E-2</v>
       </c>
       <c r="F52">
-        <f>RANK(E52,E:E,1)</f>
+        <f t="shared" si="17"/>
         <v>7</v>
       </c>
       <c r="G52">
@@ -5506,15 +5496,15 @@
         <v>2204672.88</v>
       </c>
       <c r="I52">
-        <f>H52-G52</f>
+        <f t="shared" si="11"/>
         <v>-236027.12000000011</v>
       </c>
       <c r="J52" s="5">
-        <f>IFERROR(I52/G52, 0)</f>
+        <f t="shared" si="12"/>
         <v>-9.6704683082722218E-2</v>
       </c>
       <c r="K52">
-        <f>RANK(J52,J:J,1)</f>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="L52">
@@ -5524,15 +5514,15 @@
         <v>2056835.26</v>
       </c>
       <c r="N52">
-        <f>M52-L52</f>
+        <f t="shared" si="14"/>
         <v>-264764.74</v>
       </c>
       <c r="O52" s="5">
-        <f>IFERROR(N52/L52, 0)</f>
+        <f t="shared" si="15"/>
         <v>-0.11404408166781529</v>
       </c>
       <c r="P52">
-        <f>RANK(O52,O:O,1)</f>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
     </row>
@@ -5560,15 +5550,15 @@
         <v>24</v>
       </c>
       <c r="B56">
-        <f>VLOOKUP(A56,A1:D52,4,FALSE)</f>
+        <f t="shared" ref="B56:B61" si="18">VLOOKUP(A56,A1:D52,4,FALSE)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f>VLOOKUP(A56,A2:I52,9,FALSE)</f>
+        <f t="shared" ref="C56:C61" si="19">VLOOKUP(A56,A2:I52,9,FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
-        <f>VLOOKUP(A56,A2:N52,14,FALSE)</f>
+        <f t="shared" ref="D56:D61" si="20">VLOOKUP(A56,A2:N52,14,FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5577,15 +5567,15 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f>VLOOKUP(A57,A2:D53,4,FALSE)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="C57">
-        <f>VLOOKUP(A57,A3:I53,9,FALSE)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="D57">
-        <f>VLOOKUP(A57,A3:N53,14,FALSE)</f>
+        <f t="shared" si="20"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5594,15 +5584,15 @@
         <v>32</v>
       </c>
       <c r="B58">
-        <f>VLOOKUP(A58,A3:D54,4,FALSE)</f>
+        <f t="shared" si="18"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f>VLOOKUP(A58,A4:I54,9,FALSE)</f>
+        <f t="shared" si="19"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f>VLOOKUP(A58,A4:N54,14,FALSE)</f>
+        <f t="shared" si="20"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5611,15 +5601,15 @@
         <v>38</v>
       </c>
       <c r="B59">
-        <f>VLOOKUP(A59,A4:D55,4,FALSE)</f>
+        <f t="shared" si="18"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f>VLOOKUP(A59,A5:I55,9,FALSE)</f>
+        <f t="shared" si="19"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f>VLOOKUP(A59,A5:N55,14,FALSE)</f>
+        <f t="shared" si="20"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5628,15 +5618,15 @@
         <v>39</v>
       </c>
       <c r="B60">
-        <f>VLOOKUP(A60,A5:D56,4,FALSE)</f>
+        <f t="shared" si="18"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f>VLOOKUP(A60,A6:I56,9,FALSE)</f>
+        <f t="shared" si="19"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f>VLOOKUP(A60,A6:N56,14,FALSE)</f>
+        <f t="shared" si="20"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5645,15 +5635,15 @@
         <v>55</v>
       </c>
       <c r="B61">
-        <f>VLOOKUP(A61,A6:D57,4,FALSE)</f>
+        <f t="shared" si="18"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f>VLOOKUP(A61,A7:I57,9,FALSE)</f>
+        <f t="shared" si="19"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f>VLOOKUP(A61,A7:N57,14,FALSE)</f>
+        <f t="shared" si="20"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5681,15 +5671,15 @@
         <v>24</v>
       </c>
       <c r="B65">
-        <f>_xlfn.XLOOKUP(A65,A2:A52,D2:D52)</f>
+        <f t="shared" ref="B65:B70" si="21">_xlfn.XLOOKUP(A65,A2:A52,D2:D52)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C65">
-        <f>_xlfn.XLOOKUP(A65,A2:A52,I2:I52)</f>
+        <f t="shared" ref="C65:C70" si="22">_xlfn.XLOOKUP(A65,A2:A52,I2:I52)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D65">
-        <f>_xlfn.XLOOKUP(A65,A2:A52,N2:N52)</f>
+        <f t="shared" ref="D65:D70" si="23">_xlfn.XLOOKUP(A65,A2:A52,N2:N52)</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5698,15 +5688,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f>_xlfn.XLOOKUP(A66,A3:A53,D3:D53)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="C66">
-        <f>_xlfn.XLOOKUP(A66,A3:A53,I3:I53)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="D66">
-        <f>_xlfn.XLOOKUP(A66,A3:A53,N3:N53)</f>
+        <f t="shared" si="23"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5715,15 +5705,15 @@
         <v>32</v>
       </c>
       <c r="B67">
-        <f>_xlfn.XLOOKUP(A67,A4:A54,D4:D54)</f>
+        <f t="shared" si="21"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f>_xlfn.XLOOKUP(A67,A4:A54,I4:I54)</f>
+        <f t="shared" si="22"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f>_xlfn.XLOOKUP(A67,A4:A54,N4:N54)</f>
+        <f t="shared" si="23"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5732,15 +5722,15 @@
         <v>38</v>
       </c>
       <c r="B68">
-        <f>_xlfn.XLOOKUP(A68,A5:A55,D5:D55)</f>
+        <f t="shared" si="21"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f>_xlfn.XLOOKUP(A68,A5:A55,I5:I55)</f>
+        <f t="shared" si="22"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f>_xlfn.XLOOKUP(A68,A5:A55,N5:N55)</f>
+        <f t="shared" si="23"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5749,15 +5739,15 @@
         <v>39</v>
       </c>
       <c r="B69">
-        <f>_xlfn.XLOOKUP(A69,A6:A56,D6:D56)</f>
+        <f t="shared" si="21"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f>_xlfn.XLOOKUP(A69,A6:A56,I6:I56)</f>
+        <f t="shared" si="22"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f>_xlfn.XLOOKUP(A69,A6:A56,N6:N56)</f>
+        <f t="shared" si="23"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5766,15 +5756,15 @@
         <v>55</v>
       </c>
       <c r="B70">
-        <f>_xlfn.XLOOKUP(A70,A7:A57,D7:D57)</f>
+        <f t="shared" si="21"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f>_xlfn.XLOOKUP(A70,A7:A57,I7:I57)</f>
+        <f t="shared" si="22"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f>_xlfn.XLOOKUP(A70,A7:A57,N7:N57)</f>
+        <f t="shared" si="23"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5802,15 +5792,15 @@
         <v>24</v>
       </c>
       <c r="B74">
-        <f>INDEX(D2:D52,MATCH(A74,A2:A52,1))</f>
+        <f t="shared" ref="B74:B79" si="24">INDEX(D2:D52,MATCH(A74,A2:A52,1))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C74">
-        <f>INDEX(I2:I52,MATCH(A74,A2:A52,0))</f>
+        <f t="shared" ref="C74:C79" si="25">INDEX(I2:I52,MATCH(A74,A2:A52,0))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D74">
-        <f>INDEX(N2:N52,MATCH(A74,A2:A52,0))</f>
+        <f t="shared" ref="D74:D79" si="26">INDEX(N2:N52,MATCH(A74,A2:A52,0))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5819,15 +5809,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f>INDEX(D3:D53,MATCH(A75,A3:A53,1))</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="C75">
-        <f>INDEX(I3:I53,MATCH(A75,A3:A53,0))</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="D75">
-        <f>INDEX(N3:N53,MATCH(A75,A3:A53,0))</f>
+        <f t="shared" si="26"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5836,15 +5826,15 @@
         <v>32</v>
       </c>
       <c r="B76">
-        <f>INDEX(D4:D54,MATCH(A76,A4:A54,1))</f>
+        <f t="shared" si="24"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f>INDEX(I4:I54,MATCH(A76,A4:A54,0))</f>
+        <f t="shared" si="25"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f>INDEX(N4:N54,MATCH(A76,A4:A54,0))</f>
+        <f t="shared" si="26"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5853,15 +5843,15 @@
         <v>38</v>
       </c>
       <c r="B77">
-        <f>INDEX(D5:D55,MATCH(A77,A5:A55,1))</f>
+        <f t="shared" si="24"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f>INDEX(I5:I55,MATCH(A77,A5:A55,0))</f>
+        <f t="shared" si="25"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f>INDEX(N5:N55,MATCH(A77,A5:A55,0))</f>
+        <f t="shared" si="26"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5870,15 +5860,15 @@
         <v>39</v>
       </c>
       <c r="B78">
-        <f>INDEX(D6:D56,MATCH(A78,A6:A56,1))</f>
+        <f t="shared" si="24"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f>INDEX(I6:I56,MATCH(A78,A6:A56,0))</f>
+        <f t="shared" si="25"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f>INDEX(N6:N56,MATCH(A78,A6:A56,0))</f>
+        <f t="shared" si="26"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5887,15 +5877,15 @@
         <v>55</v>
       </c>
       <c r="B79">
-        <f>INDEX(D7:D57,MATCH(A79,A7:A57,1))</f>
+        <f t="shared" si="24"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f>INDEX(I7:I57,MATCH(A79,A7:A57,0))</f>
+        <f t="shared" si="25"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f>INDEX(N7:N57,MATCH(A79,A7:A57,0))</f>
+        <f t="shared" si="26"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5922,12 +5912,12 @@
         <v>73</v>
       </c>
       <c r="B84" s="6">
-        <f>INDEX(B2:B52,MATCH(Table2[[#Headers],[Finance]],A2:A52,0))</f>
-        <v>8837300</v>
+        <f>INDEX(B2:B52,MATCH($B$87,A2:A52,0))</f>
+        <v>3329000</v>
       </c>
       <c r="C84" s="6">
-        <f>INDEX(C2:C52,MATCH(Table2[[#Headers],[Finance]],A2:A52,0))</f>
-        <v>8460963.1999999899</v>
+        <f>INDEX(C2:C52,MATCH($B$87,A2:A52,0))</f>
+        <v>2946071.21</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
@@ -5935,12 +5925,12 @@
         <v>74</v>
       </c>
       <c r="B85" s="6">
-        <f>INDEX(G2:G52, MATCH(Table2[[#Headers],[Finance]],A2:A52,0))</f>
-        <v>9713300</v>
+        <f>INDEX(G3:G53,MATCH($B$87,A3:A53,0))</f>
+        <v>3390900</v>
       </c>
       <c r="C85" s="6">
-        <f>INDEX(H2:H52,MATCH(Table2[[#Headers],[Finance]],A2:A52,))</f>
-        <v>8991707.2399999909</v>
+        <f>INDEX(H3:H53,MATCH($B$87,A3:A53,0))</f>
+        <v>3051483.41</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -5948,17 +5938,17 @@
         <v>75</v>
       </c>
       <c r="B86" s="6">
-        <f>INDEX(L2:L52,MATCH(Table2[[#Headers],[Finance]],A2:A52,))</f>
-        <v>9343000</v>
+        <f>INDEX(L4:L54,MATCH($B$87,A4:A54,0))</f>
+        <v>3345200</v>
       </c>
       <c r="C86" s="6">
-        <f>INDEX(M2:M52,MATCH(Table2[[#Headers],[Finance]],A2:A52,))</f>
-        <v>8766655.9100000001</v>
+        <f>INDEX(M4:M54,MATCH($B$87,A4:A54,0))</f>
+        <v>2946440.08</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -6095,21 +6085,15 @@
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 B87" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry!" error="Please select a department from the list" promptTitle="Departments" prompt="Select Department" sqref="B87:B88" xr:uid="{5B104185-893C-42C4-840A-72EB8FDECD55}">
-      <formula1>$A$2:$A$52</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>